<commit_message>
Se modula todo el codigo de datos generales
</commit_message>
<xml_diff>
--- a/Archivos_excel/01_Retroalimentacion/Formato_retro_PLE (20_Agosto2024).xlsx
+++ b/Archivos_excel/01_Retroalimentacion/Formato_retro_PLE (20_Agosto2024).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365inegi-my.sharepoint.com/personal/patricio_moreno_inegi_org_mx/Documents/2023-DeptoDiseño/Aplicativo ED PL/Pruebas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365inegi-my.sharepoint.com/personal/francisco_deferia_inegi_org_mx/Documents/001_Programacion_FJMD/02_C#/03_App_PLE_INEGI/Archivos_excel/01_Retroalimentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="157" documentId="8_{86DDDAAD-1804-4C2D-B692-2AD38DF1B53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6B05A36-B905-4588-8477-1CB04643ED22}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -519,40 +519,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -570,7 +536,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -580,47 +567,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -674,10 +621,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1000,7 +943,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1073,7 +1016,7 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="10">
@@ -1095,8 +1038,8 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="41">
+      <c r="A4" s="36"/>
+      <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -1113,8 +1056,8 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="41">
+      <c r="A5" s="36"/>
+      <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -1131,8 +1074,8 @@
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="41">
+      <c r="A6" s="36"/>
+      <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -1149,8 +1092,8 @@
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:12" ht="36" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="41">
+      <c r="A7" s="36"/>
+      <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -1167,14 +1110,14 @@
       <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="41">
+      <c r="A8" s="36"/>
+      <c r="B8" s="8">
         <v>6</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="16" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="16"/>
@@ -1185,8 +1128,8 @@
       <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="41">
+      <c r="A9" s="36"/>
+      <c r="B9" s="8">
         <v>7</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -1203,8 +1146,8 @@
       <c r="L9" s="14"/>
     </row>
     <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="41">
+      <c r="A10" s="36"/>
+      <c r="B10" s="8">
         <v>8</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -1221,8 +1164,8 @@
       <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" ht="36" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="41">
+      <c r="A11" s="36"/>
+      <c r="B11" s="8">
         <v>9</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1239,8 +1182,8 @@
       <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="41">
+      <c r="A12" s="36"/>
+      <c r="B12" s="8">
         <v>10</v>
       </c>
       <c r="C12" s="16" t="s">
@@ -1257,8 +1200,8 @@
       <c r="L12" s="14"/>
     </row>
     <row r="13" spans="1:12" ht="36" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
-      <c r="B13" s="41">
+      <c r="A13" s="37"/>
+      <c r="B13" s="8">
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -1275,7 +1218,7 @@
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="10">
@@ -1297,7 +1240,7 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="8">
         <v>2</v>
       </c>
@@ -1315,7 +1258,7 @@
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="8">
         <v>3</v>
       </c>
@@ -1333,7 +1276,7 @@
       <c r="L16" s="14"/>
     </row>
     <row r="17" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="8">
         <v>4</v>
       </c>
@@ -1351,7 +1294,7 @@
       <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="8">
         <v>5</v>
       </c>
@@ -1369,7 +1312,7 @@
       <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="10">
@@ -1391,7 +1334,7 @@
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="8">
         <v>2</v>
       </c>
@@ -1409,7 +1352,7 @@
       <c r="L20" s="14"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="8">
         <v>3</v>
       </c>
@@ -1427,7 +1370,7 @@
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="8">
         <v>4</v>
       </c>
@@ -1445,7 +1388,7 @@
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="8">
         <v>5</v>
       </c>
@@ -1463,7 +1406,7 @@
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="8">
         <v>6</v>
       </c>
@@ -1481,7 +1424,7 @@
       <c r="L24" s="14"/>
     </row>
     <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="8">
         <v>7</v>
       </c>
@@ -1499,27 +1442,20 @@
       <c r="L25" s="14"/>
     </row>
     <row r="26" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="8">
         <v>8</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
       <c r="L26" s="14"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="31" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="10">
@@ -1528,7 +1464,7 @@
       <c r="C27" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="28" t="s">
         <v>55</v>
       </c>
       <c r="E27" s="12"/>
@@ -1541,7 +1477,7 @@
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A28" s="32"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="8">
         <v>2</v>
       </c>
@@ -1559,7 +1495,7 @@
       <c r="L28" s="14"/>
     </row>
     <row r="29" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A29" s="32"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="8">
         <v>3</v>
       </c>
@@ -1577,7 +1513,7 @@
       <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A30" s="26"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="20">
         <v>4</v>
       </c>
@@ -1597,29 +1533,29 @@
       <c r="L30" s="15"/>
     </row>
     <row r="31" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="35">
+      <c r="B31" s="23">
         <v>1</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="39"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="27"/>
     </row>
     <row r="32" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="8">
@@ -1639,7 +1575,7 @@
       <c r="L32" s="14"/>
     </row>
     <row r="33" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="8">
         <v>2</v>
       </c>
@@ -1657,7 +1593,7 @@
       <c r="L33" s="14"/>
     </row>
     <row r="34" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="8">
         <v>3</v>
       </c>
@@ -1675,7 +1611,7 @@
       <c r="L34" s="14"/>
     </row>
     <row r="35" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="8">
         <v>4</v>
       </c>
@@ -1691,7 +1627,7 @@
       <c r="L35" s="14"/>
     </row>
     <row r="36" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A36" s="26"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="20">
         <v>5</v>
       </c>
@@ -1720,35 +1656,19 @@
     <mergeCell ref="A3:A13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E28:E35 E3:E18">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+  <conditionalFormatting sqref="E3:E25">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Completa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E22 E25">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+  <conditionalFormatting sqref="E28:E35">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>"Completa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
-      <formula>"Pendiente"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"Completa"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Pendiente"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Completa"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Observaciones Dani, Berenice terminadas.
</commit_message>
<xml_diff>
--- a/Archivos_excel/01_Retroalimentacion/Formato_retro_PLE (20_Agosto2024).xlsx
+++ b/Archivos_excel/01_Retroalimentacion/Formato_retro_PLE (20_Agosto2024).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365inegi-my.sharepoint.com/personal/patricio_moreno_inegi_org_mx/Documents/2023-DeptoDiseño/Aplicativo ED PL/Pruebas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365inegi-my.sharepoint.com/personal/jesus_barron_inegi_org_mx/Documents/Desktop/Poder lejislativos/Proyecto propuesta C#/Repositorio_GitHub/Archivos_excel/01_Retroalimentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{86DDDAAD-1804-4C2D-B692-2AD38DF1B53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6B05A36-B905-4588-8477-1CB04643ED22}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="8_{86DDDAAD-1804-4C2D-B692-2AD38DF1B53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F537B138-A448-47B1-BCDF-7C24C3C17FEC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{7D6F1DB5-4C81-46D9-BE7A-7D2828049709}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
   <si>
     <t>Hoja</t>
   </si>
@@ -265,6 +265,21 @@
   </si>
   <si>
     <t>Fecha de publicación en la Gaceta o Periódico Oficial.</t>
+  </si>
+  <si>
+    <t>Completa</t>
+  </si>
+  <si>
+    <t>Se ajusto el contenido de "Nivel escolaridad" integrando Ultimo Grado de estudios y su estatus</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Validar el tipo de recuadro</t>
+  </si>
+  <si>
+    <t>Se agustaron las variables parra el recuadro</t>
   </si>
 </sst>
 </file>
@@ -466,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -519,40 +534,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -570,7 +551,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -580,47 +582,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -674,10 +636,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -999,28 +957,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1B3382-1023-49B2-8510-518855AAFEA5}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="4"/>
-    <col min="3" max="3" width="35.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="64.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="4"/>
-    <col min="9" max="9" width="48.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="31.28515625" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="4"/>
+    <col min="2" max="2" width="11.44140625" style="4"/>
+    <col min="3" max="3" width="35.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="64.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="4"/>
+    <col min="9" max="9" width="48.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="33.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="31.33203125" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1073,7 +1031,7 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="10">
@@ -1085,7 +1043,9 @@
       <c r="D3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="17" t="s">
+        <v>74</v>
+      </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="11"/>
@@ -1095,8 +1055,8 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="41">
+      <c r="A4" s="36"/>
+      <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -1105,7 +1065,9 @@
       <c r="D4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="9"/>
@@ -1113,8 +1075,8 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="41">
+      <c r="A5" s="36"/>
+      <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -1123,7 +1085,9 @@
       <c r="D5" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="9"/>
@@ -1131,8 +1095,8 @@
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="41">
+      <c r="A6" s="36"/>
+      <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -1141,16 +1105,18 @@
       <c r="D6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:12" ht="36" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="41">
+    <row r="7" spans="1:12" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A7" s="36"/>
+      <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -1159,7 +1125,9 @@
       <c r="D7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="9"/>
@@ -1167,17 +1135,19 @@
       <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
-      <c r="B8" s="41">
+      <c r="A8" s="36"/>
+      <c r="B8" s="8">
         <v>6</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="9"/>
@@ -1185,8 +1155,8 @@
       <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="41">
+      <c r="A9" s="36"/>
+      <c r="B9" s="8">
         <v>7</v>
       </c>
       <c r="C9" s="16" t="s">
@@ -1195,16 +1165,20 @@
       <c r="D9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="E9" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="G9" s="16"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="L9" s="14"/>
     </row>
     <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="41">
+      <c r="A10" s="36"/>
+      <c r="B10" s="8">
         <v>8</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -1213,16 +1187,18 @@
       <c r="D10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:12" ht="36" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="41">
+    <row r="11" spans="1:12" ht="34.200000000000003" x14ac:dyDescent="0.2">
+      <c r="A11" s="36"/>
+      <c r="B11" s="8">
         <v>9</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1231,7 +1207,9 @@
       <c r="D11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="9"/>
@@ -1239,8 +1217,8 @@
       <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="41">
+      <c r="A12" s="36"/>
+      <c r="B12" s="8">
         <v>10</v>
       </c>
       <c r="C12" s="16" t="s">
@@ -1249,16 +1227,18 @@
       <c r="D12" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" ht="36" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
-      <c r="B13" s="41">
+    <row r="13" spans="1:12" ht="34.200000000000003" x14ac:dyDescent="0.2">
+      <c r="A13" s="37"/>
+      <c r="B13" s="8">
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -1267,7 +1247,9 @@
       <c r="D13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="9"/>
@@ -1275,7 +1257,7 @@
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="10">
@@ -1287,7 +1269,9 @@
       <c r="D14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="17" t="s">
+        <v>74</v>
+      </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="11"/>
@@ -1297,7 +1281,7 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="8">
         <v>2</v>
       </c>
@@ -1307,7 +1291,9 @@
       <c r="D15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="9"/>
@@ -1315,7 +1301,7 @@
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="8">
         <v>3</v>
       </c>
@@ -1325,7 +1311,9 @@
       <c r="D16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="16"/>
+      <c r="E16" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="9"/>
@@ -1333,7 +1321,7 @@
       <c r="L16" s="14"/>
     </row>
     <row r="17" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="8">
         <v>4</v>
       </c>
@@ -1343,15 +1331,19 @@
       <c r="D17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="E17" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>77</v>
+      </c>
       <c r="G17" s="16"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
+    <row r="18" spans="1:12" ht="45.6" x14ac:dyDescent="0.2">
+      <c r="A18" s="30"/>
       <c r="B18" s="8">
         <v>5</v>
       </c>
@@ -1361,15 +1353,19 @@
       <c r="D18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="E18" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="G18" s="16"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="10">
@@ -1381,7 +1377,9 @@
       <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="17" t="s">
+        <v>74</v>
+      </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="11"/>
@@ -1391,7 +1389,7 @@
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="8">
         <v>2</v>
       </c>
@@ -1401,7 +1399,9 @@
       <c r="D20" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="9"/>
@@ -1409,7 +1409,7 @@
       <c r="L20" s="14"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="8">
         <v>3</v>
       </c>
@@ -1419,7 +1419,9 @@
       <c r="D21" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="9"/>
@@ -1427,7 +1429,7 @@
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="8">
         <v>4</v>
       </c>
@@ -1437,7 +1439,9 @@
       <c r="D22" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="9"/>
@@ -1445,7 +1449,7 @@
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="8">
         <v>5</v>
       </c>
@@ -1455,7 +1459,9 @@
       <c r="D23" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="9"/>
@@ -1463,7 +1469,7 @@
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="8">
         <v>6</v>
       </c>
@@ -1473,15 +1479,19 @@
       <c r="D24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
+      <c r="E24" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>77</v>
+      </c>
       <c r="G24" s="16"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
+    <row r="25" spans="1:12" ht="45.6" x14ac:dyDescent="0.2">
+      <c r="A25" s="33"/>
       <c r="B25" s="8">
         <v>7</v>
       </c>
@@ -1491,7 +1501,9 @@
       <c r="D25" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="9"/>
@@ -1499,27 +1511,23 @@
       <c r="L25" s="14"/>
     </row>
     <row r="26" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="8">
         <v>8</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
+      <c r="E26" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="L26" s="14"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="31" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="10">
@@ -1528,10 +1536,12 @@
       <c r="C27" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -1540,8 +1550,8 @@
       <c r="K27" s="12"/>
       <c r="L27" s="13"/>
     </row>
-    <row r="28" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A28" s="32"/>
+    <row r="28" spans="1:12" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A28" s="29"/>
       <c r="B28" s="8">
         <v>2</v>
       </c>
@@ -1551,15 +1561,17 @@
       <c r="D28" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="16"/>
+      <c r="E28" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="L28" s="14"/>
     </row>
-    <row r="29" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:12" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A29" s="29"/>
       <c r="B29" s="8">
         <v>3</v>
       </c>
@@ -1569,15 +1581,17 @@
       <c r="D29" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="16"/>
+      <c r="E29" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="L29" s="14"/>
     </row>
-    <row r="30" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A30" s="26"/>
+    <row r="30" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="30"/>
       <c r="B30" s="20">
         <v>4</v>
       </c>
@@ -1587,7 +1601,9 @@
       <c r="D30" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="19"/>
+      <c r="E30" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
       <c r="H30" s="21"/>
@@ -1596,30 +1612,32 @@
       <c r="K30" s="18"/>
       <c r="L30" s="15"/>
     </row>
-    <row r="31" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A31" s="34" t="s">
+    <row r="31" spans="1:12" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="35">
+      <c r="B31" s="23">
         <v>1</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="39"/>
-    </row>
-    <row r="32" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
+      <c r="E31" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="27"/>
+    </row>
+    <row r="32" spans="1:12" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="8">
@@ -1631,15 +1649,17 @@
       <c r="D32" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="16"/>
+      <c r="E32" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="L32" s="14"/>
     </row>
-    <row r="33" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
+    <row r="33" spans="1:12" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A33" s="29"/>
       <c r="B33" s="8">
         <v>2</v>
       </c>
@@ -1649,15 +1669,17 @@
       <c r="D33" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="16"/>
+      <c r="E33" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
       <c r="L33" s="14"/>
     </row>
-    <row r="34" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
+    <row r="34" spans="1:12" ht="22.8" x14ac:dyDescent="0.2">
+      <c r="A34" s="29"/>
       <c r="B34" s="8">
         <v>3</v>
       </c>
@@ -1667,15 +1689,17 @@
       <c r="D34" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="16"/>
+      <c r="E34" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
       <c r="L34" s="14"/>
     </row>
-    <row r="35" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
+    <row r="35" spans="1:12" ht="34.200000000000003" x14ac:dyDescent="0.2">
+      <c r="A35" s="29"/>
       <c r="B35" s="8">
         <v>4</v>
       </c>
@@ -1685,13 +1709,15 @@
       <c r="D35" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
       <c r="L35" s="14"/>
     </row>
-    <row r="36" spans="1:12" ht="48" x14ac:dyDescent="0.2">
-      <c r="A36" s="26"/>
+    <row r="36" spans="1:12" ht="34.200000000000003" x14ac:dyDescent="0.2">
+      <c r="A36" s="30"/>
       <c r="B36" s="20">
         <v>5</v>
       </c>
@@ -1701,7 +1727,9 @@
       <c r="D36" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="18"/>
+      <c r="E36" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
@@ -1720,40 +1748,24 @@
     <mergeCell ref="A3:A13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E28:E35 E3:E18">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+  <conditionalFormatting sqref="E3:E27">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Completa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E22 E25">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+  <conditionalFormatting sqref="E28:E36">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>"Completa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
-      <formula>"Pendiente"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"Completa"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Pendiente"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Completa"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H28:H34 E28:E35 H3:H25 E3:E25" xr:uid="{32FA0E09-31A7-48C0-A844-3C55608E19D8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H28:H34 H3:H25 E3:E36" xr:uid="{32FA0E09-31A7-48C0-A844-3C55608E19D8}">
       <formula1>"Pendiente, Completa"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>